<commit_message>
Add 36413-f20, 36423-f20, 38423-f00, 38463-f00, 38473-f20, and fix 36413-f10
</commit_message>
<xml_diff>
--- a/examples/36413-f10.xlsx
+++ b/examples/36413-f10.xlsx
@@ -7452,7 +7452,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7785,9 +7785,33 @@
         <v>Maximum no. of eNB X2 GTP Transport Layer Addresses for an GTP end-point in the message. Value is 16.</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>maxnoofIRATReportingCells</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Maximum no. cells to be included. Value is 128.</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>maxnoofCandidateCells</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Maximum no. of candidate cells.</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>maxnoofCellineNB</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Maximum no. cells that can be served by an eNB. Value is 256.</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B41"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B44"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -38719,7 +38743,7 @@
 
 <file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B96"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -39252,9 +39276,169 @@
         <v>The MME does not identify any PLMN provided by the eNB.</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>HO Reporting Cause</v>
+      </c>
+      <c r="B72" t="str">
+        <v>Meaning</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Application Container Syntax Error</v>
+      </c>
+      <c r="B73" t="str">
+        <v>The Application Container IE is syntactically incorrect.</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Inconsistent Reporting Cell Identifier</v>
+      </c>
+      <c r="B74" t="str">
+        <v>- In case the reporting RAT is GERAN: the Reporting Cell Identifier in the Application Container IE does not match with the Destination Cell Identifier IE value (in the case of a RAN-INFORMATION-REQUEST PDU) or with the Source Cell Identifier IE value (in the case of a RAN-INFORMATION PDU) of the RIM header. - In case the reporting RAT is UTRAN or E-UTRAN: the cell identified by Reporting Cell Identifier in the Application Container IE is unknown in the RNC (UTRAN case) or in the eNodeB (E-UTRAN case) identified by the Destination Cell Identifier IE value in the RAN-INFORMATION-REQUEST PDU.</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>Unspecified</v>
+      </c>
+      <c r="B75" t="str">
+        <v>Sent when none of the above cause values applies.</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>Cell Activation Cause</v>
+      </c>
+      <c r="B77" t="str">
+        <v>Meaning</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>Application Container Syntax Error</v>
+      </c>
+      <c r="B78" t="str">
+        <v>The Application Container IE is syntactically incorrect.</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>Inconsistent Reporting Cell Identifier</v>
+      </c>
+      <c r="B79" t="str">
+        <v>- In case the reporting RAT is E-UTRAN: The Reporting Cell Identifier in the Application Container IE is unknown in the eNB identified by the Destination Cell Identifier IE value of the RIM header of a RAN-INFORMATION-REQUEST PDU or the reporting cell identifier in the Application Container IE does not match with the Source Cell Identifier IE value of the RIM header of a RAN-INFORMATION PDU.</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>Unspecified</v>
+      </c>
+      <c r="B80" t="str">
+        <v>Sent when none of the above cause values applies.</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>Cell State Indication Cause</v>
+      </c>
+      <c r="B82" t="str">
+        <v>Meaning</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>Application Container Syntax Error</v>
+      </c>
+      <c r="B83" t="str">
+        <v>The Application Container IE is syntactically incorrect.</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>Inconsistent Reporting Cell Identifier</v>
+      </c>
+      <c r="B84" t="str">
+        <v>- In case the reporting RAT is E-UTRAN: The Reporting Cell Identifier in the Application Container IE does not match with the Source Cell Identifier IE value of the RIM header of a RAN-INFORMATION-REQUEST PDU or the reporting cell identifier in the Application Container IE does not match with the Destination Cell Identifier IE value of the RIM header of a RAN-INFORMATION PDU.</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>Unspecified</v>
+      </c>
+      <c r="B85" t="str">
+        <v>Sent when none of the above cause values applies.</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>Failure Event Reporting Cause</v>
+      </c>
+      <c r="B87" t="str">
+        <v>Meaning</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>Application Container Syntax Error</v>
+      </c>
+      <c r="B88" t="str">
+        <v>The Application Container IE is syntactically incorrect.</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>Inconsistent Reporting Cell Identifier</v>
+      </c>
+      <c r="B89" t="str">
+        <v>- In case the reporting RAT is E-UTRAN: The Reporting Cell Identifier in the Application Container IE does not match with the Source Cell Identifier IE value of the RIM header of a RAN-INFORMATION-REQUEST PDU or the reporting cell identifier in the Application Container IE does not match with the Destination Cell Identifier IE value of the RIM header of a RAN-INFORMATION PDU.</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>Unspecified</v>
+      </c>
+      <c r="B90" t="str">
+        <v>Sent when none of the above cause values applies</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>Cell Load Reporting Cause</v>
+      </c>
+      <c r="B92" t="str">
+        <v>Meaning</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>Application Container Syntax Error</v>
+      </c>
+      <c r="B93" t="str">
+        <v>The Application Container IE is syntactically incorrect.</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>Inconsistent Reporting Cell Identifier</v>
+      </c>
+      <c r="B94" t="str">
+        <v>- In case the reporting RAT is GERAN or eHRPD: the Reporting Cell Identifier in the Application Container IE does not match with the Destination Cell Identifier IE value (in the case of a RAN-INFORMATION-REQUEST PDU) or with the Source Cell Identifier IE value (in the case of a RAN-INFORMATION PDU) of the RIM header. - In case the reporting RAT is UTRAN or E-UTRAN: the cell identified by Reporting Cell Identifier in the Application Container IE is unknown in the RNC (UTRAN case) or in the eNodeB (E-UTRAN case) identified by the Destination Cell Identifier IE value in the RAN-INFORMATION-REQUEST PDU.</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>Unspecified</v>
+      </c>
+      <c r="B95" t="str">
+        <v>Sent when none of the above cause values applies</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B71"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B96"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>